<commit_message>
sql file and excel on 28th sep 11 50 am
</commit_message>
<xml_diff>
--- a/Ecommerce API.xlsx
+++ b/Ecommerce API.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ecommerce\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF030A43-5909-4AF5-8B00-35C8956A2D9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B0DD067-E8D3-4927-8B68-11A408F7FD5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="574" xr2:uid="{9451E60B-EB0E-4489-857D-01CC188E9BE1}"/>
   </bookViews>
@@ -34,14 +34,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="223">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="222">
   <si>
     <t>Add Product</t>
   </si>
   <si>
-    <t>localhost:3000/addProduct/</t>
-  </si>
-  <si>
     <t>Edit Product</t>
   </si>
   <si>
@@ -57,21 +54,12 @@
     <t>View Product</t>
   </si>
   <si>
-    <t>localhost:3000/viewProduct/</t>
-  </si>
-  <si>
     <t>View Category</t>
   </si>
   <si>
-    <t>localhost:3000/viewCategory/</t>
-  </si>
-  <si>
     <t>Add Category</t>
   </si>
   <si>
-    <t>localhost:3000/addCategory/</t>
-  </si>
-  <si>
     <t>Edit Category</t>
   </si>
   <si>
@@ -87,15 +75,9 @@
     <t>View Brand</t>
   </si>
   <si>
-    <t>localhost:3000/viewBrand/</t>
-  </si>
-  <si>
     <t>Add Brand</t>
   </si>
   <si>
-    <t>localhost:3000/addBrand/</t>
-  </si>
-  <si>
     <t>Edit Brand</t>
   </si>
   <si>
@@ -501,9 +483,6 @@
     <t>cart_id</t>
   </si>
   <si>
-    <t>products</t>
-  </si>
-  <si>
     <t>name</t>
   </si>
   <si>
@@ -522,9 +501,6 @@
     <t>quantity_in_stock</t>
   </si>
   <si>
-    <t>uploaded_by</t>
-  </si>
-  <si>
     <t>category_id</t>
   </si>
   <si>
@@ -568,18 +544,6 @@
   </si>
   <si>
     <t>discount_id</t>
-  </si>
-  <si>
-    <t>percentage</t>
-  </si>
-  <si>
-    <t>upload_by</t>
-  </si>
-  <si>
-    <t>start_date</t>
-  </si>
-  <si>
-    <t>end_date</t>
   </si>
   <si>
     <t>discount_type</t>
@@ -754,12 +718,45 @@
   <si>
     <t>request approve</t>
   </si>
+  <si>
+    <t>CREATED</t>
+  </si>
+  <si>
+    <t>NEED TO CREATE</t>
+  </si>
+  <si>
+    <t>product</t>
+  </si>
+  <si>
+    <t>start_date_and_time</t>
+  </si>
+  <si>
+    <t>end_date_and_time</t>
+  </si>
+  <si>
+    <t>localhost:3000/addCategory</t>
+  </si>
+  <si>
+    <t>localhost:3000/viewBrand</t>
+  </si>
+  <si>
+    <t>localhost:3000/addBrand</t>
+  </si>
+  <si>
+    <t>localhost:3000/viewProduct</t>
+  </si>
+  <si>
+    <t>localhost:3000/addProduct</t>
+  </si>
+  <si>
+    <t>localhost:3000/viewCategory</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -810,8 +807,15 @@
       <name val="Consolas"/>
       <family val="3"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="9" tint="-0.499984740745262"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -836,8 +840,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -860,11 +876,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="9" tint="-0.499984740745262"/>
+      </left>
+      <right style="thin">
+        <color theme="9" tint="-0.499984740745262"/>
+      </right>
+      <top style="thin">
+        <color theme="9" tint="-0.499984740745262"/>
+      </top>
+      <bottom style="thin">
+        <color theme="9" tint="-0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -880,17 +911,20 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1385,7 +1419,7 @@
   <dimension ref="B2:I25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1403,16 +1437,16 @@
   <sheetData>
     <row r="2" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2" t="s">
-        <v>16</v>
-      </c>
-      <c r="F2" t="s">
-        <v>17</v>
+        <v>219</v>
+      </c>
+      <c r="E2" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" s="16" t="s">
+        <v>217</v>
       </c>
     </row>
     <row r="3" spans="2:9" x14ac:dyDescent="0.25">
@@ -1420,313 +1454,313 @@
         <v>0</v>
       </c>
       <c r="C3" t="s">
-        <v>1</v>
-      </c>
-      <c r="E3" t="s">
-        <v>18</v>
-      </c>
-      <c r="F3" t="s">
-        <v>19</v>
+        <v>220</v>
+      </c>
+      <c r="E3" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" s="16" t="s">
+        <v>218</v>
       </c>
     </row>
     <row r="4" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" t="s">
         <v>2</v>
       </c>
-      <c r="C4" t="s">
-        <v>3</v>
-      </c>
       <c r="E4" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="F4" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" t="s">
         <v>4</v>
       </c>
-      <c r="C5" t="s">
-        <v>5</v>
-      </c>
       <c r="E5" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="F5" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C7" t="s">
-        <v>9</v>
+      <c r="B7" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" s="16" t="s">
+        <v>221</v>
       </c>
       <c r="E7" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="F7" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="H7" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="I7" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
     </row>
     <row r="8" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B8" t="s">
-        <v>10</v>
-      </c>
-      <c r="C8" t="s">
-        <v>11</v>
+      <c r="B8" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="16" t="s">
+        <v>216</v>
       </c>
       <c r="E8" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="F8" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="H8" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="I8" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
     </row>
     <row r="9" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C9" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="E9" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="F9" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="H9" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="I9" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
     </row>
     <row r="10" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C10" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="E10" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="F10" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="H10" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="I10" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
     </row>
     <row r="12" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="C12" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="E12" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="F12" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="H12" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="I12" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
     </row>
     <row r="13" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="C13" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="E13" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="F13" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="H13" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="I13" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
     </row>
     <row r="14" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="C14" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="E14" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="F14" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="H14" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="I14" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
     </row>
     <row r="15" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="C15" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="E15" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="F15" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="H15" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="I15" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
     </row>
     <row r="17" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="C17" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="E17" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="F17" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="H17" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="I17" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
     </row>
     <row r="18" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="C18" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="E18" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="F18" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="H18" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="I18" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
     </row>
     <row r="19" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="C19" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="E19" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="F19" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="H19" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="I19" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
     </row>
     <row r="20" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="C20" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="E20" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="F20" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="H20" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="I20" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
     </row>
     <row r="22" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="C22" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
     </row>
     <row r="23" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="C23" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
     </row>
     <row r="24" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="C24" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
     </row>
     <row r="25" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="C25" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
     </row>
   </sheetData>
@@ -1759,7 +1793,7 @@
   <sheetData>
     <row r="5" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
-        <v>199</v>
+        <v>187</v>
       </c>
     </row>
   </sheetData>
@@ -1769,745 +1803,803 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8DB0B49-8369-45F4-BB0B-0C2F56F401E6}">
-  <dimension ref="A2:O28"/>
+  <dimension ref="A1:O28"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView topLeftCell="C1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.5703125" style="8" customWidth="1"/>
-    <col min="2" max="2" width="20.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.5703125" style="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.85546875" style="8" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.42578125" style="8" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.85546875" style="8" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.85546875" style="8" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.42578125" style="8" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.7109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.42578125" style="8" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="20.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="11.7109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="15.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="16" max="16384" width="9.140625" style="8"/>
+    <col min="1" max="1" width="3.28515625" style="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="5" width="17.5703125" style="7" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.85546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.5703125" style="7" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.7109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.5703125" style="7" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.85546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="20.140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="14" max="15" width="17.5703125" style="7" bestFit="1" customWidth="1"/>
+    <col min="16" max="16384" width="9.140625" style="7"/>
   </cols>
   <sheetData>
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A1" s="11"/>
+      <c r="B1" s="10" t="s">
+        <v>212</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>212</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>212</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>212</v>
+      </c>
+      <c r="F1" s="12" t="s">
+        <v>211</v>
+      </c>
+      <c r="G1" s="12" t="s">
+        <v>211</v>
+      </c>
+      <c r="H1" s="10" t="s">
+        <v>212</v>
+      </c>
+      <c r="I1" s="12" t="s">
+        <v>211</v>
+      </c>
+      <c r="J1" s="10" t="s">
+        <v>212</v>
+      </c>
+      <c r="K1" s="12" t="s">
+        <v>211</v>
+      </c>
+      <c r="L1" s="12" t="s">
+        <v>211</v>
+      </c>
+      <c r="M1" s="12" t="s">
+        <v>211</v>
+      </c>
+      <c r="N1" s="12" t="s">
+        <v>211</v>
+      </c>
+      <c r="O1" s="12" t="s">
+        <v>211</v>
+      </c>
+    </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A2" s="9"/>
-      <c r="B2" s="10">
+      <c r="A2" s="11"/>
+      <c r="B2" s="13">
         <v>1</v>
       </c>
-      <c r="C2" s="10">
+      <c r="C2" s="13">
         <v>2</v>
       </c>
-      <c r="D2" s="10">
+      <c r="D2" s="13">
         <v>3</v>
       </c>
-      <c r="E2" s="10">
+      <c r="E2" s="13">
         <v>4</v>
       </c>
-      <c r="F2" s="10">
+      <c r="F2" s="13">
         <v>5</v>
       </c>
-      <c r="G2" s="10">
+      <c r="G2" s="13">
         <v>6</v>
       </c>
-      <c r="H2" s="10">
+      <c r="H2" s="13">
         <v>7</v>
       </c>
-      <c r="I2" s="10">
+      <c r="I2" s="13">
         <v>8</v>
       </c>
-      <c r="J2" s="10">
+      <c r="J2" s="13">
         <v>9</v>
       </c>
-      <c r="K2" s="10">
+      <c r="K2" s="13">
         <v>10</v>
       </c>
-      <c r="L2" s="10">
+      <c r="L2" s="13">
         <v>11</v>
       </c>
-      <c r="M2" s="10">
+      <c r="M2" s="13">
         <v>12</v>
       </c>
-      <c r="N2" s="10">
+      <c r="N2" s="13">
         <v>13</v>
       </c>
-      <c r="O2" s="10">
+      <c r="O2" s="13">
         <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A3" s="9"/>
-      <c r="B3" s="7" t="s">
+      <c r="A3" s="11"/>
+      <c r="B3" s="14" t="s">
+        <v>116</v>
+      </c>
+      <c r="C3" s="14" t="s">
+        <v>134</v>
+      </c>
+      <c r="D3" s="14" t="s">
+        <v>140</v>
+      </c>
+      <c r="E3" s="14" t="s">
+        <v>145</v>
+      </c>
+      <c r="F3" s="14" t="s">
+        <v>152</v>
+      </c>
+      <c r="G3" s="14" t="s">
+        <v>153</v>
+      </c>
+      <c r="H3" s="14" t="s">
+        <v>147</v>
+      </c>
+      <c r="I3" s="14" t="s">
+        <v>213</v>
+      </c>
+      <c r="J3" s="14" t="s">
+        <v>157</v>
+      </c>
+      <c r="K3" s="14" t="s">
+        <v>162</v>
+      </c>
+      <c r="L3" s="14" t="s">
+        <v>133</v>
+      </c>
+      <c r="M3" s="14" t="s">
+        <v>174</v>
+      </c>
+      <c r="N3" s="14" t="s">
+        <v>168</v>
+      </c>
+      <c r="O3" s="14" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A4" s="11">
+        <v>1</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>117</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>135</v>
+      </c>
+      <c r="D4" s="11" t="s">
+        <v>141</v>
+      </c>
+      <c r="E4" s="11" t="s">
+        <v>146</v>
+      </c>
+      <c r="F4" s="11" t="s">
+        <v>155</v>
+      </c>
+      <c r="G4" s="11" t="s">
+        <v>156</v>
+      </c>
+      <c r="H4" s="11" t="s">
+        <v>148</v>
+      </c>
+      <c r="I4" s="11" t="s">
+        <v>142</v>
+      </c>
+      <c r="J4" s="11" t="s">
+        <v>158</v>
+      </c>
+      <c r="K4" s="11" t="s">
+        <v>163</v>
+      </c>
+      <c r="L4" s="11" t="s">
+        <v>166</v>
+      </c>
+      <c r="M4" s="15" t="s">
+        <v>165</v>
+      </c>
+      <c r="N4" s="11" t="s">
+        <v>169</v>
+      </c>
+      <c r="O4" s="11" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A5" s="11">
+        <v>2</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>118</v>
+      </c>
+      <c r="C5" s="11" t="s">
+        <v>117</v>
+      </c>
+      <c r="D5" s="11" t="s">
+        <v>135</v>
+      </c>
+      <c r="E5" s="11" t="s">
+        <v>142</v>
+      </c>
+      <c r="F5" s="11" t="s">
+        <v>149</v>
+      </c>
+      <c r="G5" s="11" t="s">
+        <v>149</v>
+      </c>
+      <c r="H5" s="11" t="s">
+        <v>117</v>
+      </c>
+      <c r="I5" s="11" t="s">
+        <v>149</v>
+      </c>
+      <c r="J5" s="11" t="s">
+        <v>142</v>
+      </c>
+      <c r="K5" s="11" t="s">
+        <v>164</v>
+      </c>
+      <c r="L5" s="11" t="s">
+        <v>167</v>
+      </c>
+      <c r="M5" s="11" t="s">
+        <v>118</v>
+      </c>
+      <c r="N5" s="11" t="s">
+        <v>142</v>
+      </c>
+      <c r="O5" s="11" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A6" s="11">
+        <v>3</v>
+      </c>
+      <c r="B6" s="11" t="s">
+        <v>119</v>
+      </c>
+      <c r="C6" s="11" t="s">
+        <v>136</v>
+      </c>
+      <c r="D6" s="11" t="s">
+        <v>142</v>
+      </c>
+      <c r="E6" s="11" t="s">
+        <v>117</v>
+      </c>
+      <c r="F6" s="11" t="s">
+        <v>123</v>
+      </c>
+      <c r="G6" s="11" t="s">
+        <v>123</v>
+      </c>
+      <c r="H6" s="11" t="s">
+        <v>142</v>
+      </c>
+      <c r="I6" s="11" t="s">
+        <v>150</v>
+      </c>
+      <c r="J6" s="11" t="s">
+        <v>117</v>
+      </c>
+      <c r="K6" s="11" t="s">
+        <v>166</v>
+      </c>
+      <c r="L6" s="11"/>
+      <c r="M6" s="11" t="s">
+        <v>119</v>
+      </c>
+      <c r="N6" s="11" t="s">
+        <v>166</v>
+      </c>
+      <c r="O6" s="11" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A7" s="11">
+        <v>4</v>
+      </c>
+      <c r="B7" s="11" t="s">
+        <v>120</v>
+      </c>
+      <c r="C7" s="11" t="s">
+        <v>137</v>
+      </c>
+      <c r="D7" s="11" t="s">
+        <v>143</v>
+      </c>
+      <c r="E7" s="11" t="s">
+        <v>166</v>
+      </c>
+      <c r="F7" s="11" t="s">
+        <v>166</v>
+      </c>
+      <c r="G7" s="11" t="s">
+        <v>166</v>
+      </c>
+      <c r="H7" s="11" t="s">
+        <v>143</v>
+      </c>
+      <c r="I7" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="J7" s="11" t="s">
+        <v>159</v>
+      </c>
+      <c r="K7" s="11"/>
+      <c r="L7" s="11"/>
+      <c r="M7" s="11" t="s">
+        <v>120</v>
+      </c>
+      <c r="N7" s="15" t="s">
+        <v>165</v>
+      </c>
+      <c r="O7" s="15" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A8" s="11">
+        <v>5</v>
+      </c>
+      <c r="B8" s="11" t="s">
+        <v>121</v>
+      </c>
+      <c r="C8" s="11" t="s">
+        <v>138</v>
+      </c>
+      <c r="D8" s="11" t="s">
+        <v>144</v>
+      </c>
+      <c r="E8" s="11" t="s">
+        <v>172</v>
+      </c>
+      <c r="F8" s="15" t="s">
+        <v>165</v>
+      </c>
+      <c r="G8" s="15" t="s">
+        <v>165</v>
+      </c>
+      <c r="H8" s="11" t="s">
+        <v>166</v>
+      </c>
+      <c r="I8" s="11" t="s">
+        <v>155</v>
+      </c>
+      <c r="J8" s="11" t="s">
+        <v>160</v>
+      </c>
+      <c r="K8" s="11"/>
+      <c r="L8" s="11"/>
+      <c r="M8" s="11" t="s">
+        <v>121</v>
+      </c>
+      <c r="N8" s="11" t="s">
+        <v>214</v>
+      </c>
+      <c r="O8" s="11" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A9" s="11">
+        <v>6</v>
+      </c>
+      <c r="B9" s="11" t="s">
         <v>122</v>
       </c>
-      <c r="C3" s="7" t="s">
-        <v>140</v>
-      </c>
-      <c r="D3" s="7" t="s">
-        <v>146</v>
-      </c>
-      <c r="E3" s="7" t="s">
-        <v>151</v>
-      </c>
-      <c r="F3" s="7" t="s">
-        <v>159</v>
-      </c>
-      <c r="G3" s="7" t="s">
-        <v>160</v>
-      </c>
-      <c r="H3" s="7" t="s">
-        <v>153</v>
-      </c>
-      <c r="I3" s="7" t="s">
-        <v>155</v>
-      </c>
-      <c r="J3" s="7" t="s">
+      <c r="C9" s="11" t="s">
+        <v>166</v>
+      </c>
+      <c r="D9" s="11" t="s">
+        <v>166</v>
+      </c>
+      <c r="E9" s="11" t="s">
+        <v>173</v>
+      </c>
+      <c r="F9" s="11" t="s">
+        <v>172</v>
+      </c>
+      <c r="G9" s="11" t="s">
+        <v>172</v>
+      </c>
+      <c r="H9" s="11" t="s">
+        <v>172</v>
+      </c>
+      <c r="I9" s="11" t="s">
+        <v>156</v>
+      </c>
+      <c r="J9" s="11" t="s">
+        <v>161</v>
+      </c>
+      <c r="K9" s="11"/>
+      <c r="L9" s="11"/>
+      <c r="M9" s="11" t="s">
+        <v>122</v>
+      </c>
+      <c r="N9" s="11" t="s">
+        <v>215</v>
+      </c>
+      <c r="O9" s="11" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A10" s="11">
+        <v>7</v>
+      </c>
+      <c r="B10" s="11" t="s">
+        <v>123</v>
+      </c>
+      <c r="C10" s="11" t="s">
+        <v>172</v>
+      </c>
+      <c r="D10" s="11" t="s">
+        <v>172</v>
+      </c>
+      <c r="E10" s="11"/>
+      <c r="F10" s="11" t="s">
+        <v>173</v>
+      </c>
+      <c r="G10" s="11" t="s">
+        <v>173</v>
+      </c>
+      <c r="H10" s="11" t="s">
+        <v>173</v>
+      </c>
+      <c r="I10" s="11" t="s">
+        <v>154</v>
+      </c>
+      <c r="J10" s="11" t="s">
+        <v>166</v>
+      </c>
+      <c r="K10" s="11"/>
+      <c r="L10" s="11"/>
+      <c r="M10" s="11" t="s">
+        <v>123</v>
+      </c>
+      <c r="N10" s="11" t="s">
+        <v>171</v>
+      </c>
+      <c r="O10" s="11" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A11" s="11">
+        <v>8</v>
+      </c>
+      <c r="B11" s="11" t="s">
+        <v>124</v>
+      </c>
+      <c r="C11" s="11" t="s">
+        <v>173</v>
+      </c>
+      <c r="D11" s="11" t="s">
+        <v>173</v>
+      </c>
+      <c r="E11" s="11"/>
+      <c r="F11" s="11"/>
+      <c r="G11" s="11"/>
+      <c r="H11" s="11"/>
+      <c r="I11" s="11" t="s">
+        <v>123</v>
+      </c>
+      <c r="J11" s="11" t="s">
+        <v>172</v>
+      </c>
+      <c r="K11" s="11"/>
+      <c r="L11" s="11"/>
+      <c r="M11" s="15" t="s">
         <v>165</v>
       </c>
-      <c r="K3" s="7" t="s">
-        <v>170</v>
-      </c>
-      <c r="L3" s="7" t="s">
+      <c r="N11" s="11" t="s">
+        <v>172</v>
+      </c>
+      <c r="O11" s="11"/>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A12" s="11">
+        <v>9</v>
+      </c>
+      <c r="B12" s="11" t="s">
+        <v>125</v>
+      </c>
+      <c r="C12" s="11"/>
+      <c r="D12" s="11"/>
+      <c r="E12" s="11"/>
+      <c r="F12" s="11"/>
+      <c r="G12" s="11"/>
+      <c r="H12" s="11"/>
+      <c r="I12" s="15" t="s">
+        <v>165</v>
+      </c>
+      <c r="J12" s="11" t="s">
+        <v>173</v>
+      </c>
+      <c r="K12" s="11"/>
+      <c r="L12" s="11"/>
+      <c r="M12" s="11" t="s">
         <v>139</v>
       </c>
-      <c r="M3" s="7" t="s">
-        <v>186</v>
-      </c>
-      <c r="N3" s="7" t="s">
+      <c r="N12" s="11" t="s">
+        <v>173</v>
+      </c>
+      <c r="O12" s="11"/>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A13" s="11">
+        <v>10</v>
+      </c>
+      <c r="B13" s="11" t="s">
+        <v>126</v>
+      </c>
+      <c r="C13" s="11"/>
+      <c r="D13" s="11"/>
+      <c r="E13" s="11"/>
+      <c r="F13" s="11"/>
+      <c r="G13" s="11"/>
+      <c r="H13" s="11"/>
+      <c r="I13" s="11" t="s">
+        <v>166</v>
+      </c>
+      <c r="J13" s="11"/>
+      <c r="K13" s="11"/>
+      <c r="L13" s="11"/>
+      <c r="M13" s="11" t="s">
+        <v>130</v>
+      </c>
+      <c r="N13" s="11"/>
+      <c r="O13" s="11"/>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A14" s="11">
+        <v>11</v>
+      </c>
+      <c r="B14" s="11" t="s">
+        <v>127</v>
+      </c>
+      <c r="C14" s="11"/>
+      <c r="D14" s="11"/>
+      <c r="E14" s="11"/>
+      <c r="F14" s="11"/>
+      <c r="G14" s="11"/>
+      <c r="H14" s="11"/>
+      <c r="I14" s="11" t="s">
+        <v>172</v>
+      </c>
+      <c r="J14" s="11"/>
+      <c r="K14" s="11"/>
+      <c r="L14" s="11"/>
+      <c r="M14" s="11" t="s">
+        <v>131</v>
+      </c>
+      <c r="N14" s="11"/>
+      <c r="O14" s="11"/>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A15" s="11">
+        <v>12</v>
+      </c>
+      <c r="B15" s="11" t="s">
+        <v>128</v>
+      </c>
+      <c r="C15" s="11"/>
+      <c r="D15" s="11"/>
+      <c r="E15" s="11"/>
+      <c r="F15" s="11"/>
+      <c r="G15" s="11"/>
+      <c r="H15" s="11"/>
+      <c r="I15" s="11" t="s">
+        <v>173</v>
+      </c>
+      <c r="J15" s="11"/>
+      <c r="K15" s="11"/>
+      <c r="L15" s="11"/>
+      <c r="M15" s="11" t="s">
+        <v>132</v>
+      </c>
+      <c r="N15" s="11"/>
+      <c r="O15" s="11"/>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A16" s="11">
+        <v>13</v>
+      </c>
+      <c r="B16" s="11" t="s">
+        <v>129</v>
+      </c>
+      <c r="C16" s="11"/>
+      <c r="D16" s="11"/>
+      <c r="E16" s="11"/>
+      <c r="F16" s="11"/>
+      <c r="G16" s="11"/>
+      <c r="H16" s="11"/>
+      <c r="I16" s="11"/>
+      <c r="J16" s="11"/>
+      <c r="K16" s="11"/>
+      <c r="L16" s="11"/>
+      <c r="M16" s="11" t="s">
+        <v>163</v>
+      </c>
+      <c r="N16" s="11"/>
+      <c r="O16" s="11"/>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A17" s="11">
+        <v>14</v>
+      </c>
+      <c r="B17" s="11" t="s">
+        <v>130</v>
+      </c>
+      <c r="C17" s="11"/>
+      <c r="D17" s="11"/>
+      <c r="E17" s="11"/>
+      <c r="F17" s="11"/>
+      <c r="G17" s="11"/>
+      <c r="H17" s="11"/>
+      <c r="I17" s="11"/>
+      <c r="J17" s="11"/>
+      <c r="K17" s="11"/>
+      <c r="L17" s="11"/>
+      <c r="M17" s="11" t="s">
+        <v>166</v>
+      </c>
+      <c r="N17" s="11"/>
+      <c r="O17" s="11"/>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A18" s="11">
+        <v>15</v>
+      </c>
+      <c r="B18" s="11" t="s">
+        <v>131</v>
+      </c>
+      <c r="C18" s="11"/>
+      <c r="D18" s="11"/>
+      <c r="E18" s="11"/>
+      <c r="F18" s="11"/>
+      <c r="G18" s="11"/>
+      <c r="H18" s="11"/>
+      <c r="I18" s="11"/>
+      <c r="J18" s="11"/>
+      <c r="K18" s="11"/>
+      <c r="L18" s="11"/>
+      <c r="M18" s="11" t="s">
+        <v>172</v>
+      </c>
+      <c r="N18" s="11"/>
+      <c r="O18" s="11"/>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A19" s="11">
+        <v>16</v>
+      </c>
+      <c r="B19" s="11" t="s">
+        <v>132</v>
+      </c>
+      <c r="C19" s="11"/>
+      <c r="D19" s="11"/>
+      <c r="E19" s="11"/>
+      <c r="F19" s="11"/>
+      <c r="G19" s="11"/>
+      <c r="H19" s="11"/>
+      <c r="I19" s="11"/>
+      <c r="J19" s="11"/>
+      <c r="K19" s="11"/>
+      <c r="L19" s="11"/>
+      <c r="M19" s="11" t="s">
+        <v>173</v>
+      </c>
+      <c r="N19" s="11"/>
+      <c r="O19" s="11"/>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A20" s="11">
+        <v>17</v>
+      </c>
+      <c r="B20" s="11" t="s">
+        <v>166</v>
+      </c>
+      <c r="C20" s="11"/>
+      <c r="D20" s="11"/>
+      <c r="E20" s="11"/>
+      <c r="F20" s="11"/>
+      <c r="G20" s="11"/>
+      <c r="H20" s="11"/>
+      <c r="I20" s="11"/>
+      <c r="J20" s="11"/>
+      <c r="K20" s="11"/>
+      <c r="L20" s="11"/>
+      <c r="M20" s="11"/>
+      <c r="N20" s="11"/>
+      <c r="O20" s="11"/>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A21" s="11">
+        <v>18</v>
+      </c>
+      <c r="B21" s="11" t="s">
+        <v>172</v>
+      </c>
+      <c r="C21" s="11"/>
+      <c r="D21" s="11"/>
+      <c r="E21" s="11"/>
+      <c r="F21" s="11"/>
+      <c r="G21" s="11"/>
+      <c r="H21" s="11"/>
+      <c r="I21" s="11"/>
+      <c r="J21" s="11"/>
+      <c r="K21" s="11"/>
+      <c r="L21" s="11"/>
+      <c r="M21" s="11"/>
+      <c r="N21" s="11"/>
+      <c r="O21" s="11"/>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A22" s="11">
+        <v>19</v>
+      </c>
+      <c r="B22" s="11" t="s">
+        <v>173</v>
+      </c>
+      <c r="C22" s="11"/>
+      <c r="D22" s="11"/>
+      <c r="E22" s="11"/>
+      <c r="F22" s="11"/>
+      <c r="G22" s="11"/>
+      <c r="H22" s="11"/>
+      <c r="I22" s="11"/>
+      <c r="J22" s="11"/>
+      <c r="K22" s="11"/>
+      <c r="L22" s="11"/>
+      <c r="M22" s="11"/>
+      <c r="N22" s="11"/>
+      <c r="O22" s="11"/>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="F23" s="11"/>
+      <c r="G23" s="11"/>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B25" s="7">
+        <v>0</v>
+      </c>
+      <c r="C25" s="7" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B26" s="7">
+        <v>1</v>
+      </c>
+      <c r="C26" s="7" t="s">
         <v>176</v>
       </c>
-      <c r="O3" s="7" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A4" s="9">
-        <v>1</v>
-      </c>
-      <c r="B4" s="9" t="s">
-        <v>123</v>
-      </c>
-      <c r="C4" s="9" t="s">
-        <v>141</v>
-      </c>
-      <c r="D4" s="9" t="s">
-        <v>147</v>
-      </c>
-      <c r="E4" s="9" t="s">
-        <v>152</v>
-      </c>
-      <c r="F4" s="9" t="s">
-        <v>163</v>
-      </c>
-      <c r="G4" s="9" t="s">
-        <v>164</v>
-      </c>
-      <c r="H4" s="9" t="s">
-        <v>154</v>
-      </c>
-      <c r="I4" s="9" t="s">
-        <v>148</v>
-      </c>
-      <c r="J4" s="9" t="s">
-        <v>166</v>
-      </c>
-      <c r="K4" s="9" t="s">
-        <v>171</v>
-      </c>
-      <c r="L4" s="9" t="s">
-        <v>174</v>
-      </c>
-      <c r="M4" s="11" t="s">
-        <v>173</v>
-      </c>
-      <c r="N4" s="9" t="s">
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B27" s="7">
+        <v>2</v>
+      </c>
+      <c r="C27" s="7" t="s">
         <v>177</v>
       </c>
-      <c r="O4" s="9" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A5" s="9">
-        <v>2</v>
-      </c>
-      <c r="B5" s="9" t="s">
-        <v>124</v>
-      </c>
-      <c r="C5" s="9" t="s">
-        <v>123</v>
-      </c>
-      <c r="D5" s="9" t="s">
-        <v>141</v>
-      </c>
-      <c r="E5" s="9" t="s">
-        <v>148</v>
-      </c>
-      <c r="F5" s="9" t="s">
-        <v>156</v>
-      </c>
-      <c r="G5" s="9" t="s">
-        <v>156</v>
-      </c>
-      <c r="H5" s="9" t="s">
-        <v>123</v>
-      </c>
-      <c r="I5" s="9" t="s">
-        <v>156</v>
-      </c>
-      <c r="J5" s="9" t="s">
-        <v>148</v>
-      </c>
-      <c r="K5" s="9" t="s">
-        <v>172</v>
-      </c>
-      <c r="L5" s="9" t="s">
-        <v>175</v>
-      </c>
-      <c r="M5" s="9" t="s">
-        <v>124</v>
-      </c>
-      <c r="N5" s="9" t="s">
-        <v>148</v>
-      </c>
-      <c r="O5" s="9" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A6" s="9">
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B28" s="7">
         <v>3</v>
       </c>
-      <c r="B6" s="9" t="s">
-        <v>125</v>
-      </c>
-      <c r="C6" s="9" t="s">
-        <v>142</v>
-      </c>
-      <c r="D6" s="9" t="s">
-        <v>148</v>
-      </c>
-      <c r="E6" s="9" t="s">
-        <v>123</v>
-      </c>
-      <c r="F6" s="9" t="s">
-        <v>129</v>
-      </c>
-      <c r="G6" s="9" t="s">
-        <v>129</v>
-      </c>
-      <c r="H6" s="9" t="s">
-        <v>148</v>
-      </c>
-      <c r="I6" s="9" t="s">
-        <v>157</v>
-      </c>
-      <c r="J6" s="9" t="s">
-        <v>123</v>
-      </c>
-      <c r="K6" s="9" t="s">
-        <v>174</v>
-      </c>
-      <c r="L6" s="9"/>
-      <c r="M6" s="9" t="s">
-        <v>125</v>
-      </c>
-      <c r="N6" s="9" t="s">
-        <v>174</v>
-      </c>
-      <c r="O6" s="9" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A7" s="9">
-        <v>4</v>
-      </c>
-      <c r="B7" s="9" t="s">
-        <v>126</v>
-      </c>
-      <c r="C7" s="9" t="s">
-        <v>143</v>
-      </c>
-      <c r="D7" s="9" t="s">
-        <v>149</v>
-      </c>
-      <c r="E7" s="9" t="s">
-        <v>174</v>
-      </c>
-      <c r="F7" s="9" t="s">
-        <v>174</v>
-      </c>
-      <c r="G7" s="9" t="s">
-        <v>174</v>
-      </c>
-      <c r="H7" s="9" t="s">
-        <v>149</v>
-      </c>
-      <c r="I7" s="9" t="s">
-        <v>158</v>
-      </c>
-      <c r="J7" s="9" t="s">
-        <v>167</v>
-      </c>
-      <c r="K7" s="9"/>
-      <c r="L7" s="9"/>
-      <c r="M7" s="9" t="s">
-        <v>126</v>
-      </c>
-      <c r="N7" s="9" t="s">
+      <c r="C28" s="7" t="s">
         <v>178</v>
       </c>
-      <c r="O7" s="9" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A8" s="9">
-        <v>5</v>
-      </c>
-      <c r="B8" s="9" t="s">
-        <v>127</v>
-      </c>
-      <c r="C8" s="9" t="s">
-        <v>144</v>
-      </c>
-      <c r="D8" s="9" t="s">
-        <v>150</v>
-      </c>
-      <c r="E8" s="9" t="s">
-        <v>184</v>
-      </c>
-      <c r="F8" s="9" t="s">
-        <v>184</v>
-      </c>
-      <c r="G8" s="9" t="s">
-        <v>184</v>
-      </c>
-      <c r="H8" s="9" t="s">
-        <v>174</v>
-      </c>
-      <c r="I8" s="9" t="s">
-        <v>163</v>
-      </c>
-      <c r="J8" s="9" t="s">
-        <v>168</v>
-      </c>
-      <c r="K8" s="9"/>
-      <c r="L8" s="9"/>
-      <c r="M8" s="9" t="s">
-        <v>127</v>
-      </c>
-      <c r="N8" s="9" t="s">
-        <v>180</v>
-      </c>
-      <c r="O8" s="9" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A9" s="9">
-        <v>6</v>
-      </c>
-      <c r="B9" s="9" t="s">
-        <v>128</v>
-      </c>
-      <c r="C9" s="9" t="s">
-        <v>174</v>
-      </c>
-      <c r="D9" s="9" t="s">
-        <v>174</v>
-      </c>
-      <c r="E9" s="9" t="s">
-        <v>185</v>
-      </c>
-      <c r="F9" s="9" t="s">
-        <v>185</v>
-      </c>
-      <c r="G9" s="9" t="s">
-        <v>185</v>
-      </c>
-      <c r="H9" s="9" t="s">
-        <v>184</v>
-      </c>
-      <c r="I9" s="9" t="s">
-        <v>164</v>
-      </c>
-      <c r="J9" s="9" t="s">
-        <v>169</v>
-      </c>
-      <c r="K9" s="9"/>
-      <c r="L9" s="9"/>
-      <c r="M9" s="9" t="s">
-        <v>128</v>
-      </c>
-      <c r="N9" s="9" t="s">
-        <v>181</v>
-      </c>
-      <c r="O9" s="9"/>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A10" s="9">
-        <v>7</v>
-      </c>
-      <c r="B10" s="9" t="s">
-        <v>129</v>
-      </c>
-      <c r="C10" s="9" t="s">
-        <v>184</v>
-      </c>
-      <c r="D10" s="9" t="s">
-        <v>184</v>
-      </c>
-      <c r="E10" s="9"/>
-      <c r="F10" s="9"/>
-      <c r="G10" s="9"/>
-      <c r="H10" s="9" t="s">
-        <v>185</v>
-      </c>
-      <c r="I10" s="9" t="s">
-        <v>161</v>
-      </c>
-      <c r="J10" s="9" t="s">
-        <v>174</v>
-      </c>
-      <c r="K10" s="9"/>
-      <c r="L10" s="9"/>
-      <c r="M10" s="9" t="s">
-        <v>129</v>
-      </c>
-      <c r="N10" s="9" t="s">
-        <v>183</v>
-      </c>
-      <c r="O10" s="9"/>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A11" s="9">
-        <v>8</v>
-      </c>
-      <c r="B11" s="9" t="s">
-        <v>130</v>
-      </c>
-      <c r="C11" s="9" t="s">
-        <v>185</v>
-      </c>
-      <c r="D11" s="9" t="s">
-        <v>185</v>
-      </c>
-      <c r="E11" s="9"/>
-      <c r="F11" s="9"/>
-      <c r="G11" s="9"/>
-      <c r="H11" s="9"/>
-      <c r="I11" s="9" t="s">
-        <v>129</v>
-      </c>
-      <c r="J11" s="9" t="s">
-        <v>184</v>
-      </c>
-      <c r="K11" s="9"/>
-      <c r="L11" s="9"/>
-      <c r="M11" s="9" t="s">
-        <v>179</v>
-      </c>
-      <c r="N11" s="9"/>
-      <c r="O11" s="9"/>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A12" s="9">
-        <v>9</v>
-      </c>
-      <c r="B12" s="9" t="s">
-        <v>131</v>
-      </c>
-      <c r="C12" s="9"/>
-      <c r="D12" s="9"/>
-      <c r="E12" s="9"/>
-      <c r="F12" s="9"/>
-      <c r="G12" s="9"/>
-      <c r="H12" s="9"/>
-      <c r="I12" s="9" t="s">
-        <v>162</v>
-      </c>
-      <c r="J12" s="9" t="s">
-        <v>185</v>
-      </c>
-      <c r="K12" s="9"/>
-      <c r="L12" s="9"/>
-      <c r="M12" s="9" t="s">
-        <v>145</v>
-      </c>
-      <c r="N12" s="9"/>
-      <c r="O12" s="9"/>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A13" s="9">
-        <v>10</v>
-      </c>
-      <c r="B13" s="9" t="s">
-        <v>132</v>
-      </c>
-      <c r="C13" s="9"/>
-      <c r="D13" s="9"/>
-      <c r="E13" s="9"/>
-      <c r="F13" s="9"/>
-      <c r="G13" s="9"/>
-      <c r="H13" s="9"/>
-      <c r="I13" s="9" t="s">
-        <v>174</v>
-      </c>
-      <c r="J13" s="9"/>
-      <c r="K13" s="9"/>
-      <c r="L13" s="9"/>
-      <c r="M13" s="9" t="s">
-        <v>136</v>
-      </c>
-      <c r="N13" s="9"/>
-      <c r="O13" s="9"/>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A14" s="9">
-        <v>11</v>
-      </c>
-      <c r="B14" s="9" t="s">
-        <v>133</v>
-      </c>
-      <c r="C14" s="9"/>
-      <c r="D14" s="9"/>
-      <c r="E14" s="9"/>
-      <c r="F14" s="9"/>
-      <c r="G14" s="9"/>
-      <c r="H14" s="9"/>
-      <c r="I14" s="9" t="s">
-        <v>184</v>
-      </c>
-      <c r="J14" s="9"/>
-      <c r="K14" s="9"/>
-      <c r="L14" s="9"/>
-      <c r="M14" s="9" t="s">
-        <v>137</v>
-      </c>
-      <c r="N14" s="9"/>
-      <c r="O14" s="9"/>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A15" s="9">
-        <v>12</v>
-      </c>
-      <c r="B15" s="9" t="s">
-        <v>134</v>
-      </c>
-      <c r="C15" s="9"/>
-      <c r="D15" s="9"/>
-      <c r="E15" s="9"/>
-      <c r="F15" s="9"/>
-      <c r="G15" s="9"/>
-      <c r="H15" s="9"/>
-      <c r="I15" s="9" t="s">
-        <v>185</v>
-      </c>
-      <c r="J15" s="9"/>
-      <c r="K15" s="9"/>
-      <c r="L15" s="9"/>
-      <c r="M15" s="9" t="s">
-        <v>138</v>
-      </c>
-      <c r="N15" s="9"/>
-      <c r="O15" s="9"/>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A16" s="9">
-        <v>13</v>
-      </c>
-      <c r="B16" s="9" t="s">
-        <v>135</v>
-      </c>
-      <c r="C16" s="9"/>
-      <c r="D16" s="9"/>
-      <c r="E16" s="9"/>
-      <c r="F16" s="9"/>
-      <c r="G16" s="9"/>
-      <c r="H16" s="9"/>
-      <c r="I16" s="9"/>
-      <c r="J16" s="9"/>
-      <c r="K16" s="9"/>
-      <c r="L16" s="9"/>
-      <c r="M16" s="9" t="s">
-        <v>171</v>
-      </c>
-      <c r="N16" s="9"/>
-      <c r="O16" s="9"/>
-    </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A17" s="9">
-        <v>14</v>
-      </c>
-      <c r="B17" s="9" t="s">
-        <v>136</v>
-      </c>
-      <c r="C17" s="9"/>
-      <c r="D17" s="9"/>
-      <c r="E17" s="9"/>
-      <c r="F17" s="9"/>
-      <c r="G17" s="9"/>
-      <c r="H17" s="9"/>
-      <c r="I17" s="9"/>
-      <c r="J17" s="9"/>
-      <c r="K17" s="9"/>
-      <c r="L17" s="9"/>
-      <c r="M17" s="9" t="s">
-        <v>174</v>
-      </c>
-      <c r="N17" s="9"/>
-      <c r="O17" s="9"/>
-    </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A18" s="9">
-        <v>15</v>
-      </c>
-      <c r="B18" s="9" t="s">
-        <v>137</v>
-      </c>
-      <c r="C18" s="9"/>
-      <c r="D18" s="9"/>
-      <c r="E18" s="9"/>
-      <c r="F18" s="9"/>
-      <c r="G18" s="9"/>
-      <c r="H18" s="9"/>
-      <c r="I18" s="9"/>
-      <c r="J18" s="9"/>
-      <c r="K18" s="9"/>
-      <c r="L18" s="9"/>
-      <c r="M18" s="9" t="s">
-        <v>184</v>
-      </c>
-      <c r="N18" s="9"/>
-      <c r="O18" s="9"/>
-    </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A19" s="9">
-        <v>16</v>
-      </c>
-      <c r="B19" s="9" t="s">
-        <v>138</v>
-      </c>
-      <c r="C19" s="9"/>
-      <c r="D19" s="9"/>
-      <c r="E19" s="9"/>
-      <c r="F19" s="9"/>
-      <c r="G19" s="9"/>
-      <c r="H19" s="9"/>
-      <c r="I19" s="9"/>
-      <c r="J19" s="9"/>
-      <c r="K19" s="9"/>
-      <c r="L19" s="9"/>
-      <c r="M19" s="9" t="s">
-        <v>185</v>
-      </c>
-      <c r="N19" s="9"/>
-      <c r="O19" s="9"/>
-    </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A20" s="9">
-        <v>17</v>
-      </c>
-      <c r="B20" s="9" t="s">
-        <v>174</v>
-      </c>
-      <c r="C20" s="9"/>
-      <c r="D20" s="9"/>
-      <c r="E20" s="9"/>
-      <c r="F20" s="9"/>
-      <c r="G20" s="9"/>
-      <c r="H20" s="9"/>
-      <c r="I20" s="9"/>
-      <c r="J20" s="9"/>
-      <c r="K20" s="9"/>
-      <c r="L20" s="9"/>
-      <c r="M20" s="9"/>
-      <c r="N20" s="9"/>
-      <c r="O20" s="9"/>
-    </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A21" s="9">
-        <v>18</v>
-      </c>
-      <c r="B21" s="9" t="s">
-        <v>184</v>
-      </c>
-      <c r="C21" s="9"/>
-      <c r="D21" s="9"/>
-      <c r="E21" s="9"/>
-      <c r="F21" s="9"/>
-      <c r="G21" s="9"/>
-      <c r="H21" s="9"/>
-      <c r="I21" s="9"/>
-      <c r="J21" s="9"/>
-      <c r="K21" s="9"/>
-      <c r="L21" s="9"/>
-      <c r="M21" s="9"/>
-      <c r="N21" s="9"/>
-      <c r="O21" s="9"/>
-    </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A22" s="9">
-        <v>19</v>
-      </c>
-      <c r="B22" s="9" t="s">
-        <v>185</v>
-      </c>
-      <c r="C22" s="9"/>
-      <c r="D22" s="9"/>
-      <c r="E22" s="9"/>
-      <c r="F22" s="9"/>
-      <c r="G22" s="9"/>
-      <c r="H22" s="9"/>
-      <c r="I22" s="9"/>
-      <c r="J22" s="9"/>
-      <c r="K22" s="9"/>
-      <c r="L22" s="9"/>
-      <c r="M22" s="9"/>
-      <c r="N22" s="9"/>
-      <c r="O22" s="9"/>
-    </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B25" s="8">
-        <v>0</v>
-      </c>
-      <c r="C25" s="8" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B26" s="8">
-        <v>1</v>
-      </c>
-      <c r="C26" s="8" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B27" s="8">
-        <v>2</v>
-      </c>
-      <c r="C27" s="8" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B28" s="8">
-        <v>3</v>
-      </c>
-      <c r="C28" s="8" t="s">
-        <v>190</v>
-      </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A1:XFD7 I8:XFD12 A8:H1048576 M13:M19 I13:L1048576 N13:XFD1048576 M23:M1048576">
+  <conditionalFormatting sqref="M13:M19 I13:L1048576 M23:M1048576 A8:H1048576 N13:N1048576 O8:XFD1048576 I8:N12 A1:XFD7">
     <cfRule type="containsText" dxfId="8" priority="1" operator="containsText" text="cart_id">
       <formula>NOT(ISERROR(SEARCH("cart_id",A1)))</formula>
     </cfRule>
@@ -2556,59 +2648,59 @@
   <sheetData>
     <row r="4" spans="3:10" x14ac:dyDescent="0.25">
       <c r="H4" t="s">
-        <v>211</v>
+        <v>199</v>
       </c>
       <c r="J4" t="s">
-        <v>219</v>
+        <v>207</v>
       </c>
     </row>
     <row r="5" spans="3:10" x14ac:dyDescent="0.25">
       <c r="H5" t="s">
-        <v>217</v>
+        <v>205</v>
       </c>
       <c r="J5" t="s">
-        <v>222</v>
+        <v>210</v>
       </c>
     </row>
     <row r="6" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C6" t="s">
-        <v>209</v>
+        <v>197</v>
       </c>
       <c r="H6" t="s">
-        <v>218</v>
+        <v>206</v>
       </c>
     </row>
     <row r="7" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C7" t="s">
-        <v>210</v>
+        <v>198</v>
       </c>
       <c r="D7" t="s">
-        <v>211</v>
+        <v>199</v>
       </c>
       <c r="E7" t="s">
-        <v>212</v>
+        <v>200</v>
       </c>
       <c r="H7" t="s">
-        <v>220</v>
+        <v>208</v>
       </c>
     </row>
     <row r="8" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C8" t="s">
-        <v>213</v>
+        <v>201</v>
       </c>
       <c r="D8" t="s">
-        <v>215</v>
+        <v>203</v>
       </c>
       <c r="H8" t="s">
-        <v>221</v>
+        <v>209</v>
       </c>
     </row>
     <row r="9" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C9" t="s">
-        <v>214</v>
+        <v>202</v>
       </c>
       <c r="D9" t="s">
-        <v>216</v>
+        <v>204</v>
       </c>
     </row>
   </sheetData>
@@ -2628,7 +2720,7 @@
   <sheetData>
     <row r="2" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
     </row>
     <row r="3" spans="2:4" x14ac:dyDescent="0.25">
@@ -2636,10 +2728,10 @@
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="D3" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.25">
@@ -2647,10 +2739,10 @@
         <v>2</v>
       </c>
       <c r="C4" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="D4" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.25">
@@ -2658,10 +2750,10 @@
         <v>3</v>
       </c>
       <c r="C5" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="D5" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.25">
@@ -2669,10 +2761,10 @@
         <v>4</v>
       </c>
       <c r="C6" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="D6" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
     </row>
     <row r="7" spans="2:4" x14ac:dyDescent="0.25">
@@ -2680,10 +2772,10 @@
         <v>5</v>
       </c>
       <c r="C7" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="D7" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
     </row>
     <row r="8" spans="2:4" x14ac:dyDescent="0.25">
@@ -2691,10 +2783,10 @@
         <v>6</v>
       </c>
       <c r="C8" t="s">
+        <v>90</v>
+      </c>
+      <c r="D8" t="s">
         <v>96</v>
-      </c>
-      <c r="D8" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="9" spans="2:4" x14ac:dyDescent="0.25">
@@ -2702,7 +2794,7 @@
         <v>7</v>
       </c>
       <c r="C9" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
     </row>
   </sheetData>
@@ -2726,10 +2818,10 @@
   <sheetData>
     <row r="3" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.25">
@@ -2737,7 +2829,7 @@
         <v>1</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.25">
@@ -2745,10 +2837,10 @@
         <v>2</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="D5" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.25">
@@ -2756,7 +2848,7 @@
         <v>3</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
     </row>
     <row r="7" spans="2:4" x14ac:dyDescent="0.25">
@@ -2780,7 +2872,7 @@
         <v>2</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
     </row>
     <row r="12" spans="2:4" x14ac:dyDescent="0.25">
@@ -2788,7 +2880,7 @@
         <v>3</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
     </row>
     <row r="13" spans="2:4" x14ac:dyDescent="0.25">
@@ -2796,7 +2888,7 @@
         <v>4</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
     </row>
     <row r="14" spans="2:4" x14ac:dyDescent="0.25">
@@ -2804,7 +2896,7 @@
         <v>5</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
     </row>
     <row r="15" spans="2:4" x14ac:dyDescent="0.25">
@@ -2812,7 +2904,7 @@
         <v>6</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
     </row>
   </sheetData>
@@ -2838,16 +2930,16 @@
   <sheetData>
     <row r="2" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
     </row>
     <row r="3" spans="2:11" x14ac:dyDescent="0.25">
@@ -2861,7 +2953,7 @@
         <v>1</v>
       </c>
       <c r="E3" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
     </row>
     <row r="4" spans="2:11" x14ac:dyDescent="0.25">
@@ -2872,7 +2964,7 @@
         <v>2</v>
       </c>
       <c r="E4" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
     </row>
     <row r="5" spans="2:11" x14ac:dyDescent="0.25">
@@ -2883,7 +2975,7 @@
         <v>3</v>
       </c>
       <c r="E5" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
     </row>
     <row r="6" spans="2:11" x14ac:dyDescent="0.25">
@@ -2894,7 +2986,7 @@
         <v>4</v>
       </c>
       <c r="E6" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
     </row>
     <row r="7" spans="2:11" x14ac:dyDescent="0.25">
@@ -2908,89 +3000,89 @@
         <v>1</v>
       </c>
       <c r="E7" t="s">
-        <v>191</v>
+        <v>179</v>
       </c>
     </row>
     <row r="8" spans="2:11" x14ac:dyDescent="0.25">
       <c r="D8" s="1">
         <v>2</v>
       </c>
-      <c r="E8" s="12" t="s">
+      <c r="E8" s="8" t="s">
+        <v>180</v>
+      </c>
+      <c r="F8" s="8" t="s">
+        <v>185</v>
+      </c>
+      <c r="G8" s="8" t="s">
+        <v>186</v>
+      </c>
+      <c r="H8" s="8" t="s">
+        <v>191</v>
+      </c>
+      <c r="I8" s="8" t="s">
         <v>192</v>
       </c>
-      <c r="F8" s="12" t="s">
-        <v>197</v>
-      </c>
-      <c r="G8" s="12" t="s">
-        <v>198</v>
-      </c>
-      <c r="H8" s="12" t="s">
-        <v>203</v>
-      </c>
-      <c r="I8" s="12" t="s">
-        <v>204</v>
-      </c>
-      <c r="J8" s="12" t="s">
-        <v>205</v>
-      </c>
-      <c r="K8" s="12" t="s">
-        <v>208</v>
+      <c r="J8" s="8" t="s">
+        <v>193</v>
+      </c>
+      <c r="K8" s="8" t="s">
+        <v>196</v>
       </c>
     </row>
     <row r="9" spans="2:11" x14ac:dyDescent="0.25">
       <c r="D9" s="1">
         <v>3</v>
       </c>
-      <c r="E9" s="12" t="s">
-        <v>193</v>
-      </c>
-      <c r="F9" s="12" t="s">
-        <v>197</v>
-      </c>
-      <c r="G9" s="12" t="s">
-        <v>198</v>
+      <c r="E9" s="8" t="s">
+        <v>181</v>
+      </c>
+      <c r="F9" s="8" t="s">
+        <v>185</v>
+      </c>
+      <c r="G9" s="8" t="s">
+        <v>186</v>
       </c>
     </row>
     <row r="10" spans="2:11" x14ac:dyDescent="0.25">
       <c r="D10" s="1">
         <v>4</v>
       </c>
-      <c r="E10" s="12" t="s">
-        <v>196</v>
-      </c>
-      <c r="F10" s="12" t="s">
-        <v>197</v>
-      </c>
-      <c r="G10" s="12" t="s">
-        <v>198</v>
+      <c r="E10" s="8" t="s">
+        <v>184</v>
+      </c>
+      <c r="F10" s="8" t="s">
+        <v>185</v>
+      </c>
+      <c r="G10" s="8" t="s">
+        <v>186</v>
       </c>
     </row>
     <row r="11" spans="2:11" x14ac:dyDescent="0.25">
       <c r="D11" s="1">
         <v>5</v>
       </c>
-      <c r="E11" s="12" t="s">
-        <v>194</v>
-      </c>
-      <c r="F11" s="12" t="s">
-        <v>197</v>
-      </c>
-      <c r="G11" s="12" t="s">
-        <v>198</v>
+      <c r="E11" s="8" t="s">
+        <v>182</v>
+      </c>
+      <c r="F11" s="8" t="s">
+        <v>185</v>
+      </c>
+      <c r="G11" s="8" t="s">
+        <v>186</v>
       </c>
     </row>
     <row r="12" spans="2:11" x14ac:dyDescent="0.25">
       <c r="D12" s="1">
         <v>6</v>
       </c>
-      <c r="E12" s="12" t="s">
-        <v>195</v>
-      </c>
-      <c r="F12" s="12" t="s">
-        <v>197</v>
-      </c>
-      <c r="G12" s="12" t="s">
-        <v>198</v>
+      <c r="E12" s="8" t="s">
+        <v>183</v>
+      </c>
+      <c r="F12" s="8" t="s">
+        <v>185</v>
+      </c>
+      <c r="G12" s="8" t="s">
+        <v>186</v>
       </c>
     </row>
   </sheetData>
@@ -3028,7 +3120,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>200</v>
+        <v>188</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="45" x14ac:dyDescent="0.25">
@@ -3036,18 +3128,18 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>201</v>
-      </c>
-      <c r="D2" s="13" t="s">
-        <v>202</v>
+        <v>189</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>190</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="C3" t="s">
-        <v>206</v>
-      </c>
-      <c r="D3" s="13" t="s">
-        <v>207</v>
+        <v>194</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>195</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Edit view completed for brand module
</commit_message>
<xml_diff>
--- a/Ecommerce API.xlsx
+++ b/Ecommerce API.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ecommerce\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A676C603-933B-4CF0-9299-0D26CFED457B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BB9DA18-6B1E-4ACA-BB1D-6D814F27EDB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="574" activeTab="2" xr2:uid="{9451E60B-EB0E-4489-857D-01CC188E9BE1}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="222">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="224">
   <si>
     <t>Add Product</t>
   </si>
@@ -750,6 +750,12 @@
   </si>
   <si>
     <t>localhost:3000/viewCategory</t>
+  </si>
+  <si>
+    <t>View single brand</t>
+  </si>
+  <si>
+    <t>localhost:3000/viewBrandById</t>
   </si>
 </sst>
 </file>
@@ -1419,7 +1425,7 @@
   <dimension ref="B2:I25"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1470,11 +1476,11 @@
       <c r="C4" t="s">
         <v>2</v>
       </c>
-      <c r="E4" t="s">
-        <v>14</v>
-      </c>
-      <c r="F4" t="s">
-        <v>15</v>
+      <c r="E4" s="16" t="s">
+        <v>222</v>
+      </c>
+      <c r="F4" s="16" t="s">
+        <v>223</v>
       </c>
     </row>
     <row r="5" spans="2:9" x14ac:dyDescent="0.25">
@@ -1485,9 +1491,17 @@
         <v>4</v>
       </c>
       <c r="E5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="E6" t="s">
         <v>16</v>
       </c>
-      <c r="F5" t="s">
+      <c r="F6" t="s">
         <v>17</v>
       </c>
     </row>
@@ -1498,12 +1512,6 @@
       <c r="C7" s="16" t="s">
         <v>221</v>
       </c>
-      <c r="E7" t="s">
-        <v>26</v>
-      </c>
-      <c r="F7" t="s">
-        <v>27</v>
-      </c>
       <c r="H7" t="s">
         <v>74</v>
       </c>
@@ -1519,10 +1527,10 @@
         <v>216</v>
       </c>
       <c r="E8" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F8" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="H8" t="s">
         <v>76</v>
@@ -1539,10 +1547,10 @@
         <v>9</v>
       </c>
       <c r="E9" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F9" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="H9" t="s">
         <v>78</v>
@@ -1559,16 +1567,24 @@
         <v>11</v>
       </c>
       <c r="E10" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="F10" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="H10" t="s">
         <v>80</v>
       </c>
       <c r="I10" t="s">
         <v>81</v>
+      </c>
+    </row>
+    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="E11" t="s">
+        <v>32</v>
+      </c>
+      <c r="F11" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="12" spans="2:9" x14ac:dyDescent="0.25">
@@ -1578,12 +1594,6 @@
       <c r="C12" t="s">
         <v>34</v>
       </c>
-      <c r="E12" t="s">
-        <v>18</v>
-      </c>
-      <c r="F12" t="s">
-        <v>19</v>
-      </c>
       <c r="H12" t="s">
         <v>66</v>
       </c>
@@ -1599,10 +1609,10 @@
         <v>37</v>
       </c>
       <c r="E13" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="F13" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="H13" t="s">
         <v>68</v>
@@ -1619,10 +1629,10 @@
         <v>39</v>
       </c>
       <c r="E14" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="F14" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="H14" t="s">
         <v>70</v>
@@ -1639,16 +1649,24 @@
         <v>41</v>
       </c>
       <c r="E15" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="F15" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="H15" t="s">
         <v>72</v>
       </c>
       <c r="I15" t="s">
         <v>73</v>
+      </c>
+    </row>
+    <row r="16" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="E16" t="s">
+        <v>24</v>
+      </c>
+      <c r="F16" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="17" spans="2:9" x14ac:dyDescent="0.25">
@@ -1658,12 +1676,6 @@
       <c r="C17" t="s">
         <v>43</v>
       </c>
-      <c r="E17" t="s">
-        <v>50</v>
-      </c>
-      <c r="F17" t="s">
-        <v>51</v>
-      </c>
       <c r="H17" t="s">
         <v>58</v>
       </c>
@@ -1679,10 +1691,10 @@
         <v>45</v>
       </c>
       <c r="E18" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="F18" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="H18" t="s">
         <v>60</v>
@@ -1699,10 +1711,10 @@
         <v>47</v>
       </c>
       <c r="E19" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="F19" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="H19" t="s">
         <v>62</v>
@@ -1719,16 +1731,24 @@
         <v>49</v>
       </c>
       <c r="E20" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F20" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="H20" t="s">
         <v>64</v>
       </c>
       <c r="I20" t="s">
         <v>65</v>
+      </c>
+    </row>
+    <row r="21" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="E21" t="s">
+        <v>56</v>
+      </c>
+      <c r="F21" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="22" spans="2:9" x14ac:dyDescent="0.25">
@@ -1806,7 +1826,7 @@
   <dimension ref="A1:O28"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8:G8"/>
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
backend file arrange for brand, product, category
</commit_message>
<xml_diff>
--- a/Ecommerce API.xlsx
+++ b/Ecommerce API.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ecommerce\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BB9DA18-6B1E-4ACA-BB1D-6D814F27EDB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE587B35-8661-4091-83AD-5355631A77E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="574" activeTab="2" xr2:uid="{9451E60B-EB0E-4489-857D-01CC188E9BE1}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="574" xr2:uid="{9451E60B-EB0E-4489-857D-01CC188E9BE1}"/>
   </bookViews>
   <sheets>
     <sheet name="API" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="224">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="225">
   <si>
     <t>Add Product</t>
   </si>
@@ -42,15 +42,9 @@
     <t>Edit Product</t>
   </si>
   <si>
-    <t>localhost:3000/editProduct/id</t>
-  </si>
-  <si>
     <t xml:space="preserve">Delete Product </t>
   </si>
   <si>
-    <t>localhost:3000/deleteProduct/id</t>
-  </si>
-  <si>
     <t>View Product</t>
   </si>
   <si>
@@ -79,9 +73,6 @@
   </si>
   <si>
     <t>Edit Brand</t>
-  </si>
-  <si>
-    <t>localhost:3000/editBrand/id</t>
   </si>
   <si>
     <t xml:space="preserve">Delete Brand </t>
@@ -757,12 +748,25 @@
   <si>
     <t>localhost:3000/viewBrandById</t>
   </si>
+  <si>
+    <t>localhost:3000/editBrandById</t>
+  </si>
+  <si>
+    <t>Note: yellow background "completed status" 
+red background "inprogress status"</t>
+  </si>
+  <si>
+    <t>localhost:3000/editProductById</t>
+  </si>
+  <si>
+    <t>localhost:3000/deleteProductById</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -820,8 +824,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="20"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -855,6 +866,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -901,7 +924,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -931,6 +954,10 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1422,10 +1449,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9ED5812E-70CE-4E27-B25C-3893C195368C}">
-  <dimension ref="B2:I25"/>
+  <dimension ref="B1:I27"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1441,349 +1468,370 @@
     <col min="9" max="9" width="32.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="1" spans="2:9" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C1" s="18" t="s">
+        <v>222</v>
+      </c>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
+    </row>
     <row r="2" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" t="s">
-        <v>219</v>
-      </c>
-      <c r="E2" s="16" t="s">
-        <v>12</v>
-      </c>
-      <c r="F2" s="16" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" t="s">
-        <v>220</v>
-      </c>
-      <c r="E3" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="F3" s="16" t="s">
-        <v>218</v>
-      </c>
+      <c r="C2" s="18"/>
+      <c r="D2" s="18"/>
+      <c r="E2" s="18"/>
+      <c r="F2" s="18"/>
+      <c r="G2" s="18"/>
+      <c r="H2" s="18"/>
     </row>
     <row r="4" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>2</v>
+        <v>216</v>
       </c>
       <c r="E4" s="16" t="s">
-        <v>222</v>
+        <v>10</v>
       </c>
       <c r="F4" s="16" t="s">
-        <v>223</v>
+        <v>214</v>
       </c>
     </row>
     <row r="5" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C5" t="s">
+        <v>217</v>
+      </c>
+      <c r="E5" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5" s="16" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" t="s">
+        <v>223</v>
+      </c>
+      <c r="E6" s="16" t="s">
+        <v>219</v>
+      </c>
+      <c r="F6" s="16" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>2</v>
+      </c>
+      <c r="C7" t="s">
+        <v>224</v>
+      </c>
+      <c r="E7" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="F7" s="17" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="E8" t="s">
+        <v>13</v>
+      </c>
+      <c r="F8" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B9" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="E5" t="s">
-        <v>14</v>
-      </c>
-      <c r="F5" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="E6" t="s">
-        <v>16</v>
-      </c>
-      <c r="F6" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B7" s="16" t="s">
+      <c r="C9" s="16" t="s">
+        <v>218</v>
+      </c>
+      <c r="H9" t="s">
+        <v>71</v>
+      </c>
+      <c r="I9" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B10" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10" s="16" t="s">
+        <v>213</v>
+      </c>
+      <c r="E10" t="s">
+        <v>23</v>
+      </c>
+      <c r="F10" t="s">
+        <v>24</v>
+      </c>
+      <c r="H10" t="s">
+        <v>73</v>
+      </c>
+      <c r="I10" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="16" t="s">
-        <v>221</v>
-      </c>
-      <c r="H7" t="s">
-        <v>74</v>
-      </c>
-      <c r="I7" t="s">
+      <c r="C11" t="s">
+        <v>7</v>
+      </c>
+      <c r="E11" t="s">
+        <v>25</v>
+      </c>
+      <c r="F11" t="s">
+        <v>26</v>
+      </c>
+      <c r="H11" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B8" s="16" t="s">
-        <v>7</v>
-      </c>
-      <c r="C8" s="16" t="s">
-        <v>216</v>
-      </c>
-      <c r="E8" t="s">
-        <v>26</v>
-      </c>
-      <c r="F8" t="s">
-        <v>27</v>
-      </c>
-      <c r="H8" t="s">
+      <c r="I11" t="s">
         <v>76</v>
-      </c>
-      <c r="I8" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B9" t="s">
-        <v>8</v>
-      </c>
-      <c r="C9" t="s">
-        <v>9</v>
-      </c>
-      <c r="E9" t="s">
-        <v>28</v>
-      </c>
-      <c r="F9" t="s">
-        <v>29</v>
-      </c>
-      <c r="H9" t="s">
-        <v>78</v>
-      </c>
-      <c r="I9" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
-        <v>10</v>
-      </c>
-      <c r="C10" t="s">
-        <v>11</v>
-      </c>
-      <c r="E10" t="s">
-        <v>30</v>
-      </c>
-      <c r="F10" t="s">
-        <v>31</v>
-      </c>
-      <c r="H10" t="s">
-        <v>80</v>
-      </c>
-      <c r="I10" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="E11" t="s">
-        <v>32</v>
-      </c>
-      <c r="F11" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="12" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="C12" t="s">
-        <v>34</v>
+        <v>9</v>
+      </c>
+      <c r="E12" t="s">
+        <v>27</v>
+      </c>
+      <c r="F12" t="s">
+        <v>28</v>
       </c>
       <c r="H12" t="s">
-        <v>66</v>
+        <v>77</v>
       </c>
       <c r="I12" t="s">
-        <v>67</v>
+        <v>78</v>
       </c>
     </row>
     <row r="13" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B13" t="s">
-        <v>36</v>
-      </c>
-      <c r="C13" t="s">
-        <v>37</v>
-      </c>
       <c r="E13" t="s">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="F13" t="s">
-        <v>19</v>
-      </c>
-      <c r="H13" t="s">
-        <v>68</v>
-      </c>
-      <c r="I13" t="s">
-        <v>69</v>
+        <v>30</v>
       </c>
     </row>
     <row r="14" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="C14" t="s">
-        <v>39</v>
-      </c>
-      <c r="E14" t="s">
-        <v>20</v>
-      </c>
-      <c r="F14" t="s">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="H14" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="I14" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
     </row>
     <row r="15" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="C15" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="E15" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="F15" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="H15" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="I15" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
     </row>
     <row r="16" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>35</v>
+      </c>
+      <c r="C16" t="s">
+        <v>36</v>
+      </c>
       <c r="E16" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="F16" t="s">
-        <v>25</v>
+        <v>18</v>
+      </c>
+      <c r="H16" t="s">
+        <v>67</v>
+      </c>
+      <c r="I16" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="17" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="C17" t="s">
-        <v>43</v>
+        <v>38</v>
+      </c>
+      <c r="E17" t="s">
+        <v>19</v>
+      </c>
+      <c r="F17" t="s">
+        <v>20</v>
       </c>
       <c r="H17" t="s">
-        <v>58</v>
+        <v>69</v>
       </c>
       <c r="I17" t="s">
-        <v>59</v>
+        <v>70</v>
       </c>
     </row>
     <row r="18" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B18" t="s">
-        <v>44</v>
-      </c>
-      <c r="C18" t="s">
-        <v>45</v>
-      </c>
       <c r="E18" t="s">
-        <v>50</v>
+        <v>21</v>
       </c>
       <c r="F18" t="s">
-        <v>51</v>
-      </c>
-      <c r="H18" t="s">
-        <v>60</v>
-      </c>
-      <c r="I18" t="s">
-        <v>61</v>
+        <v>22</v>
       </c>
     </row>
     <row r="19" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="C19" t="s">
-        <v>47</v>
-      </c>
-      <c r="E19" t="s">
-        <v>52</v>
-      </c>
-      <c r="F19" t="s">
-        <v>53</v>
+        <v>40</v>
       </c>
       <c r="H19" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="I19" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
     </row>
     <row r="20" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
+        <v>41</v>
+      </c>
+      <c r="C20" t="s">
+        <v>42</v>
+      </c>
+      <c r="E20" t="s">
+        <v>47</v>
+      </c>
+      <c r="F20" t="s">
         <v>48</v>
       </c>
-      <c r="C20" t="s">
+      <c r="H20" t="s">
+        <v>57</v>
+      </c>
+      <c r="I20" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="21" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>43</v>
+      </c>
+      <c r="C21" t="s">
+        <v>44</v>
+      </c>
+      <c r="E21" t="s">
         <v>49</v>
       </c>
-      <c r="E20" t="s">
-        <v>54</v>
-      </c>
-      <c r="F20" t="s">
-        <v>55</v>
-      </c>
-      <c r="H20" t="s">
-        <v>64</v>
-      </c>
-      <c r="I20" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="21" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="E21" t="s">
-        <v>56</v>
-      </c>
       <c r="F21" t="s">
-        <v>57</v>
+        <v>50</v>
+      </c>
+      <c r="H21" t="s">
+        <v>59</v>
+      </c>
+      <c r="I21" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="22" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
-        <v>82</v>
+        <v>45</v>
       </c>
       <c r="C22" t="s">
-        <v>83</v>
+        <v>46</v>
+      </c>
+      <c r="E22" t="s">
+        <v>51</v>
+      </c>
+      <c r="F22" t="s">
+        <v>52</v>
+      </c>
+      <c r="H22" t="s">
+        <v>61</v>
+      </c>
+      <c r="I22" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="23" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B23" t="s">
-        <v>84</v>
-      </c>
-      <c r="C23" t="s">
-        <v>85</v>
+      <c r="E23" t="s">
+        <v>53</v>
+      </c>
+      <c r="F23" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="24" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="C24" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
     </row>
     <row r="25" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="C25" t="s">
-        <v>89</v>
+        <v>82</v>
+      </c>
+    </row>
+    <row r="26" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B26" t="s">
+        <v>83</v>
+      </c>
+      <c r="C26" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="27" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B27" t="s">
+        <v>85</v>
+      </c>
+      <c r="C27" t="s">
+        <v>86</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="C1:H2"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -1813,7 +1861,7 @@
   <sheetData>
     <row r="5" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
     </row>
   </sheetData>
@@ -1825,7 +1873,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8DB0B49-8369-45F4-BB0B-0C2F56F401E6}">
   <dimension ref="A1:O28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView topLeftCell="C1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
@@ -1849,46 +1897,46 @@
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="11"/>
       <c r="B1" s="10" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="C1" s="10" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="D1" s="10" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="E1" s="10" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="F1" s="12" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="G1" s="12" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="H1" s="10" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="I1" s="12" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="J1" s="10" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="K1" s="12" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="L1" s="12" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="M1" s="12" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="N1" s="12" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="O1" s="12" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
@@ -1939,46 +1987,46 @@
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="11"/>
       <c r="B3" s="14" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="D3" s="14" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="E3" s="14" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="F3" s="14" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="G3" s="14" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="H3" s="14" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="I3" s="14" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="J3" s="14" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="K3" s="14" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="L3" s="14" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="M3" s="14" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="N3" s="14" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="O3" s="14" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
@@ -1986,46 +2034,46 @@
         <v>1</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="D4" s="11" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="E4" s="11" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="F4" s="11" t="s">
+        <v>152</v>
+      </c>
+      <c r="G4" s="11" t="s">
+        <v>153</v>
+      </c>
+      <c r="H4" s="11" t="s">
+        <v>145</v>
+      </c>
+      <c r="I4" s="11" t="s">
+        <v>139</v>
+      </c>
+      <c r="J4" s="11" t="s">
         <v>155</v>
       </c>
-      <c r="G4" s="11" t="s">
-        <v>156</v>
-      </c>
-      <c r="H4" s="11" t="s">
-        <v>148</v>
-      </c>
-      <c r="I4" s="11" t="s">
-        <v>142</v>
-      </c>
-      <c r="J4" s="11" t="s">
-        <v>158</v>
-      </c>
       <c r="K4" s="11" t="s">
+        <v>160</v>
+      </c>
+      <c r="L4" s="11" t="s">
         <v>163</v>
       </c>
-      <c r="L4" s="11" t="s">
+      <c r="M4" s="15" t="s">
+        <v>162</v>
+      </c>
+      <c r="N4" s="11" t="s">
         <v>166</v>
       </c>
-      <c r="M4" s="15" t="s">
-        <v>165</v>
-      </c>
-      <c r="N4" s="11" t="s">
-        <v>169</v>
-      </c>
       <c r="O4" s="11" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
@@ -2033,46 +2081,46 @@
         <v>2</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="D5" s="11" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="E5" s="11" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="F5" s="11" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="G5" s="11" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="H5" s="11" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="I5" s="11" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="J5" s="11" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="K5" s="11" t="s">
+        <v>161</v>
+      </c>
+      <c r="L5" s="11" t="s">
         <v>164</v>
       </c>
-      <c r="L5" s="11" t="s">
-        <v>167</v>
-      </c>
       <c r="M5" s="11" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="N5" s="11" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="O5" s="11" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
@@ -2080,44 +2128,44 @@
         <v>3</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="D6" s="11" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="E6" s="11" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="F6" s="11" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="G6" s="11" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="H6" s="11" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="I6" s="11" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="J6" s="11" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="K6" s="11" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="L6" s="11"/>
       <c r="M6" s="11" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="N6" s="11" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="O6" s="11" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
@@ -2125,42 +2173,42 @@
         <v>4</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="D7" s="11" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="E7" s="11" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="F7" s="11" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="G7" s="11" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="H7" s="11" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="I7" s="11" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="J7" s="11" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="K7" s="11"/>
       <c r="L7" s="11"/>
       <c r="M7" s="11" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="N7" s="15" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="O7" s="15" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
@@ -2168,42 +2216,42 @@
         <v>5</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="D8" s="11" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="E8" s="11" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="F8" s="15" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="G8" s="15" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="H8" s="11" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="I8" s="11" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="J8" s="11" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="K8" s="11"/>
       <c r="L8" s="11"/>
       <c r="M8" s="11" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="N8" s="11" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="O8" s="11" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
@@ -2211,42 +2259,42 @@
         <v>6</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="D9" s="11" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="E9" s="11" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="F9" s="11" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="G9" s="11" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="H9" s="11" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="I9" s="11" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="J9" s="11" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="K9" s="11"/>
       <c r="L9" s="11"/>
       <c r="M9" s="11" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="N9" s="11" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="O9" s="11" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
@@ -2254,40 +2302,40 @@
         <v>7</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="D10" s="11" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="E10" s="11"/>
       <c r="F10" s="11" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="G10" s="11" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="H10" s="11" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="I10" s="11" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="J10" s="11" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="K10" s="11"/>
       <c r="L10" s="11"/>
       <c r="M10" s="11" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="N10" s="11" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="O10" s="11" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
@@ -2295,31 +2343,31 @@
         <v>8</v>
       </c>
       <c r="B11" s="11" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="C11" s="11" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="D11" s="11" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="E11" s="11"/>
       <c r="F11" s="11"/>
       <c r="G11" s="11"/>
       <c r="H11" s="11"/>
       <c r="I11" s="11" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="J11" s="11" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="K11" s="11"/>
       <c r="L11" s="11"/>
       <c r="M11" s="15" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="N11" s="11" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="O11" s="11"/>
     </row>
@@ -2328,7 +2376,7 @@
         <v>9</v>
       </c>
       <c r="B12" s="11" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="C12" s="11"/>
       <c r="D12" s="11"/>
@@ -2337,18 +2385,18 @@
       <c r="G12" s="11"/>
       <c r="H12" s="11"/>
       <c r="I12" s="15" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="J12" s="11" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="K12" s="11"/>
       <c r="L12" s="11"/>
       <c r="M12" s="11" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="N12" s="11" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="O12" s="11"/>
     </row>
@@ -2357,7 +2405,7 @@
         <v>10</v>
       </c>
       <c r="B13" s="11" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="C13" s="11"/>
       <c r="D13" s="11"/>
@@ -2366,13 +2414,13 @@
       <c r="G13" s="11"/>
       <c r="H13" s="11"/>
       <c r="I13" s="11" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="J13" s="11"/>
       <c r="K13" s="11"/>
       <c r="L13" s="11"/>
       <c r="M13" s="11" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="N13" s="11"/>
       <c r="O13" s="11"/>
@@ -2382,7 +2430,7 @@
         <v>11</v>
       </c>
       <c r="B14" s="11" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="C14" s="11"/>
       <c r="D14" s="11"/>
@@ -2391,13 +2439,13 @@
       <c r="G14" s="11"/>
       <c r="H14" s="11"/>
       <c r="I14" s="11" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="J14" s="11"/>
       <c r="K14" s="11"/>
       <c r="L14" s="11"/>
       <c r="M14" s="11" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="N14" s="11"/>
       <c r="O14" s="11"/>
@@ -2407,7 +2455,7 @@
         <v>12</v>
       </c>
       <c r="B15" s="11" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="C15" s="11"/>
       <c r="D15" s="11"/>
@@ -2416,13 +2464,13 @@
       <c r="G15" s="11"/>
       <c r="H15" s="11"/>
       <c r="I15" s="11" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="J15" s="11"/>
       <c r="K15" s="11"/>
       <c r="L15" s="11"/>
       <c r="M15" s="11" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="N15" s="11"/>
       <c r="O15" s="11"/>
@@ -2432,7 +2480,7 @@
         <v>13</v>
       </c>
       <c r="B16" s="11" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="C16" s="11"/>
       <c r="D16" s="11"/>
@@ -2445,7 +2493,7 @@
       <c r="K16" s="11"/>
       <c r="L16" s="11"/>
       <c r="M16" s="11" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="N16" s="11"/>
       <c r="O16" s="11"/>
@@ -2455,7 +2503,7 @@
         <v>14</v>
       </c>
       <c r="B17" s="11" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="C17" s="11"/>
       <c r="D17" s="11"/>
@@ -2468,7 +2516,7 @@
       <c r="K17" s="11"/>
       <c r="L17" s="11"/>
       <c r="M17" s="11" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="N17" s="11"/>
       <c r="O17" s="11"/>
@@ -2478,7 +2526,7 @@
         <v>15</v>
       </c>
       <c r="B18" s="11" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="C18" s="11"/>
       <c r="D18" s="11"/>
@@ -2491,7 +2539,7 @@
       <c r="K18" s="11"/>
       <c r="L18" s="11"/>
       <c r="M18" s="11" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="N18" s="11"/>
       <c r="O18" s="11"/>
@@ -2501,7 +2549,7 @@
         <v>16</v>
       </c>
       <c r="B19" s="11" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="C19" s="11"/>
       <c r="D19" s="11"/>
@@ -2514,7 +2562,7 @@
       <c r="K19" s="11"/>
       <c r="L19" s="11"/>
       <c r="M19" s="11" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="N19" s="11"/>
       <c r="O19" s="11"/>
@@ -2524,7 +2572,7 @@
         <v>17</v>
       </c>
       <c r="B20" s="11" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="C20" s="11"/>
       <c r="D20" s="11"/>
@@ -2545,7 +2593,7 @@
         <v>18</v>
       </c>
       <c r="B21" s="11" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="C21" s="11"/>
       <c r="D21" s="11"/>
@@ -2566,7 +2614,7 @@
         <v>19</v>
       </c>
       <c r="B22" s="11" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="C22" s="11"/>
       <c r="D22" s="11"/>
@@ -2591,7 +2639,7 @@
         <v>0</v>
       </c>
       <c r="C25" s="7" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.25">
@@ -2599,7 +2647,7 @@
         <v>1</v>
       </c>
       <c r="C26" s="7" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.25">
@@ -2607,7 +2655,7 @@
         <v>2</v>
       </c>
       <c r="C27" s="7" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.25">
@@ -2615,7 +2663,7 @@
         <v>3</v>
       </c>
       <c r="C28" s="7" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
     </row>
   </sheetData>
@@ -2668,59 +2716,59 @@
   <sheetData>
     <row r="4" spans="3:10" x14ac:dyDescent="0.25">
       <c r="H4" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="J4" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
     </row>
     <row r="5" spans="3:10" x14ac:dyDescent="0.25">
       <c r="H5" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="J5" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
     </row>
     <row r="6" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C6" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="H6" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
     </row>
     <row r="7" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C7" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="D7" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="E7" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="H7" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
     </row>
     <row r="8" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C8" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="D8" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="H8" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
     </row>
     <row r="9" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C9" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="D9" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
     </row>
   </sheetData>
@@ -2740,7 +2788,7 @@
   <sheetData>
     <row r="2" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
     </row>
     <row r="3" spans="2:4" x14ac:dyDescent="0.25">
@@ -2748,10 +2796,10 @@
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="D3" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.25">
@@ -2759,10 +2807,10 @@
         <v>2</v>
       </c>
       <c r="C4" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="D4" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.25">
@@ -2770,10 +2818,10 @@
         <v>3</v>
       </c>
       <c r="C5" t="s">
+        <v>87</v>
+      </c>
+      <c r="D5" t="s">
         <v>90</v>
-      </c>
-      <c r="D5" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.25">
@@ -2781,10 +2829,10 @@
         <v>4</v>
       </c>
       <c r="C6" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="D6" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
     </row>
     <row r="7" spans="2:4" x14ac:dyDescent="0.25">
@@ -2792,10 +2840,10 @@
         <v>5</v>
       </c>
       <c r="C7" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="D7" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
     </row>
     <row r="8" spans="2:4" x14ac:dyDescent="0.25">
@@ -2803,10 +2851,10 @@
         <v>6</v>
       </c>
       <c r="C8" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="D8" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
     </row>
     <row r="9" spans="2:4" x14ac:dyDescent="0.25">
@@ -2814,7 +2862,7 @@
         <v>7</v>
       </c>
       <c r="C9" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
     </row>
   </sheetData>
@@ -2838,10 +2886,10 @@
   <sheetData>
     <row r="3" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.25">
@@ -2849,7 +2897,7 @@
         <v>1</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.25">
@@ -2857,10 +2905,10 @@
         <v>2</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="D5" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.25">
@@ -2868,7 +2916,7 @@
         <v>3</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
     </row>
     <row r="7" spans="2:4" x14ac:dyDescent="0.25">
@@ -2892,7 +2940,7 @@
         <v>2</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
     </row>
     <row r="12" spans="2:4" x14ac:dyDescent="0.25">
@@ -2900,7 +2948,7 @@
         <v>3</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
     </row>
     <row r="13" spans="2:4" x14ac:dyDescent="0.25">
@@ -2908,7 +2956,7 @@
         <v>4</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="14" spans="2:4" x14ac:dyDescent="0.25">
@@ -2916,7 +2964,7 @@
         <v>5</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="15" spans="2:4" x14ac:dyDescent="0.25">
@@ -2924,7 +2972,7 @@
         <v>6</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
     </row>
   </sheetData>
@@ -2950,16 +2998,16 @@
   <sheetData>
     <row r="2" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>107</v>
-      </c>
       <c r="D2" s="1" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
     </row>
     <row r="3" spans="2:11" x14ac:dyDescent="0.25">
@@ -2973,7 +3021,7 @@
         <v>1</v>
       </c>
       <c r="E3" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
     </row>
     <row r="4" spans="2:11" x14ac:dyDescent="0.25">
@@ -2984,7 +3032,7 @@
         <v>2</v>
       </c>
       <c r="E4" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="5" spans="2:11" x14ac:dyDescent="0.25">
@@ -2995,7 +3043,7 @@
         <v>3</v>
       </c>
       <c r="E5" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="6" spans="2:11" x14ac:dyDescent="0.25">
@@ -3006,7 +3054,7 @@
         <v>4</v>
       </c>
       <c r="E6" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
     </row>
     <row r="7" spans="2:11" x14ac:dyDescent="0.25">
@@ -3020,7 +3068,7 @@
         <v>1</v>
       </c>
       <c r="E7" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
     </row>
     <row r="8" spans="2:11" x14ac:dyDescent="0.25">
@@ -3028,25 +3076,25 @@
         <v>2</v>
       </c>
       <c r="E8" s="8" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="F8" s="8" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="G8" s="8" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="H8" s="8" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="I8" s="8" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="J8" s="8" t="s">
+        <v>190</v>
+      </c>
+      <c r="K8" s="8" t="s">
         <v>193</v>
-      </c>
-      <c r="K8" s="8" t="s">
-        <v>196</v>
       </c>
     </row>
     <row r="9" spans="2:11" x14ac:dyDescent="0.25">
@@ -3054,13 +3102,13 @@
         <v>3</v>
       </c>
       <c r="E9" s="8" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="F9" s="8" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="G9" s="8" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
     </row>
     <row r="10" spans="2:11" x14ac:dyDescent="0.25">
@@ -3068,13 +3116,13 @@
         <v>4</v>
       </c>
       <c r="E10" s="8" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="F10" s="8" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="G10" s="8" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
     </row>
     <row r="11" spans="2:11" x14ac:dyDescent="0.25">
@@ -3082,13 +3130,13 @@
         <v>5</v>
       </c>
       <c r="E11" s="8" t="s">
+        <v>179</v>
+      </c>
+      <c r="F11" s="8" t="s">
         <v>182</v>
       </c>
-      <c r="F11" s="8" t="s">
-        <v>185</v>
-      </c>
       <c r="G11" s="8" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
     </row>
     <row r="12" spans="2:11" x14ac:dyDescent="0.25">
@@ -3096,13 +3144,13 @@
         <v>6</v>
       </c>
       <c r="E12" s="8" t="s">
+        <v>180</v>
+      </c>
+      <c r="F12" s="8" t="s">
+        <v>182</v>
+      </c>
+      <c r="G12" s="8" t="s">
         <v>183</v>
-      </c>
-      <c r="F12" s="8" t="s">
-        <v>185</v>
-      </c>
-      <c r="G12" s="8" t="s">
-        <v>186</v>
       </c>
     </row>
   </sheetData>
@@ -3140,7 +3188,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="45" x14ac:dyDescent="0.25">
@@ -3148,18 +3196,18 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="C3" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
     </row>
   </sheetData>

</xml_diff>